<commit_message>
Update getAvailabilityScore for design by contract
</commit_message>
<xml_diff>
--- a/Jonathan WhiteBoxTest.xlsx
+++ b/Jonathan WhiteBoxTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Github Projects\02161-Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB655C85-F2E7-4B24-880F-C88301A75688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDBC13B-A8C1-4981-A4A1-DDCFE25F53EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="62625" yWindow="9345" windowWidth="23880" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57390" yWindow="9585" windowWidth="29010" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -474,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>